<commit_message>
refactored logic tascs before first demo
</commit_message>
<xml_diff>
--- a/Tests for Comments application.xlsx
+++ b/Tests for Comments application.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7350" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="6" r:id="rId1"/>
@@ -1657,6 +1657,99 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1675,27 +1768,78 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1705,93 +1849,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1812,93 +1899,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2493,13 +2493,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2371725</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>26593</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2523,8 +2523,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1143000" y="5629275"/>
-          <a:ext cx="5495925" cy="2857500"/>
+          <a:off x="1143000" y="5629274"/>
+          <a:ext cx="6591300" cy="3427019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2852,7 +2852,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2862,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:Q15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2872,457 +2872,452 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="80"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="111"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="82"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="112"/>
+      <c r="Q3" s="113"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="81"/>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="82"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="113"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="81"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="82"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="113"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="82"/>
+      <c r="B6" s="112"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="112"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="112"/>
+      <c r="M6" s="112"/>
+      <c r="N6" s="112"/>
+      <c r="O6" s="112"/>
+      <c r="P6" s="112"/>
+      <c r="Q6" s="113"/>
     </row>
     <row r="7" spans="1:17" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85" t="s">
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>301</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="105" t="s">
         <v>168</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="84"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="105"/>
+      <c r="O8" s="105"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="105"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>302</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="84"/>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="84"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+      <c r="M9" s="105"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="105"/>
+      <c r="Q9" s="105"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>303</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="105" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="84"/>
-      <c r="O10" s="84"/>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="84"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="105"/>
+      <c r="M10" s="105"/>
+      <c r="N10" s="105"/>
+      <c r="O10" s="105"/>
+      <c r="P10" s="105"/>
+      <c r="Q10" s="105"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>304</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="105" t="s">
         <v>171</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="84"/>
-      <c r="M11" s="84"/>
-      <c r="N11" s="84"/>
-      <c r="O11" s="84"/>
-      <c r="P11" s="84"/>
-      <c r="Q11" s="84"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="105"/>
+      <c r="N11" s="105"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="105"/>
+      <c r="Q11" s="105"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>305</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="105" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="84"/>
-      <c r="M12" s="84"/>
-      <c r="N12" s="84"/>
-      <c r="O12" s="84"/>
-      <c r="P12" s="84"/>
-      <c r="Q12" s="84"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="105"/>
+      <c r="N12" s="105"/>
+      <c r="O12" s="105"/>
+      <c r="P12" s="105"/>
+      <c r="Q12" s="105"/>
     </row>
     <row r="13" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="87"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="87"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="84"/>
-      <c r="O14" s="84"/>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="84"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="105"/>
+      <c r="N14" s="105"/>
+      <c r="O14" s="105"/>
+      <c r="P14" s="105"/>
+      <c r="Q14" s="105"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="84"/>
-      <c r="O15" s="84"/>
-      <c r="P15" s="84"/>
-      <c r="Q15" s="84"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="105"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="105"/>
+      <c r="Q15" s="105"/>
     </row>
     <row r="16" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="85"/>
-      <c r="K16" s="85"/>
-      <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
-      <c r="P16" s="85"/>
-      <c r="Q16" s="85"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="107"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="108" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="88"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-      <c r="M17" s="88"/>
-      <c r="N17" s="88"/>
-      <c r="O17" s="88"/>
-      <c r="P17" s="88"/>
-      <c r="Q17" s="88"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
+      <c r="J17" s="108"/>
+      <c r="K17" s="108"/>
+      <c r="L17" s="108"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="108"/>
+      <c r="Q17" s="108"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="88"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="88"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="88"/>
-      <c r="Q18" s="88"/>
+      <c r="A18" s="108"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="108"/>
+      <c r="K18" s="108"/>
+      <c r="L18" s="108"/>
+      <c r="M18" s="108"/>
+      <c r="N18" s="108"/>
+      <c r="O18" s="108"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="88"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="88"/>
+      <c r="A19" s="108"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="108"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
+      <c r="Q19" s="108"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
+      <c r="A20" s="108"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="108"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="108"/>
+      <c r="N20" s="108"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="108"/>
+      <c r="Q20" s="108"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="88"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="88"/>
-      <c r="N21" s="88"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="88"/>
-      <c r="Q21" s="88"/>
+      <c r="A21" s="108"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="108"/>
+      <c r="J21" s="108"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="108"/>
+      <c r="N21" s="108"/>
+      <c r="O21" s="108"/>
+      <c r="P21" s="108"/>
+      <c r="Q21" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B14:Q14"/>
-    <mergeCell ref="B15:Q15"/>
-    <mergeCell ref="A13:Q13"/>
-    <mergeCell ref="A16:Q16"/>
-    <mergeCell ref="A17:Q21"/>
     <mergeCell ref="A2:Q5"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B8:M8"/>
@@ -3338,6 +3333,11 @@
     <mergeCell ref="N11:Q11"/>
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="B14:Q14"/>
+    <mergeCell ref="B15:Q15"/>
+    <mergeCell ref="A13:Q13"/>
+    <mergeCell ref="A16:Q16"/>
+    <mergeCell ref="A17:Q21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1"/>
@@ -3437,8 +3437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3457,142 +3457,142 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="90">
+      <c r="B1" s="137">
         <v>301</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="139" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="138" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="130">
+      <c r="B6" s="142">
         <v>42857</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="139" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
     </row>
     <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="99" t="s">
+      <c r="D11" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="100"/>
-      <c r="F11" s="101"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="124"/>
     </row>
     <row r="12" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="96"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="98"/>
+      <c r="A12" s="119"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
       <c r="D12" s="33" t="s">
         <v>17</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="42"/>
-      <c r="F13" s="154">
+      <c r="F13" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -3629,7 +3629,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="42"/>
-      <c r="F14" s="154">
+      <c r="F14" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="42"/>
-      <c r="F15" s="154">
+      <c r="F15" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -3659,7 +3659,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="29"/>
-      <c r="F16" s="155">
+      <c r="F16" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -3675,7 +3675,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="29"/>
-      <c r="F17" s="155">
+      <c r="F17" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -3691,7 +3691,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="29"/>
-      <c r="F18" s="155">
+      <c r="F18" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="29"/>
-      <c r="F19" s="155">
+      <c r="F19" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -3723,7 +3723,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="29"/>
-      <c r="F20" s="155">
+      <c r="F20" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -3739,7 +3739,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="29"/>
-      <c r="F21" s="155">
+      <c r="F21" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -3757,7 +3757,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="47"/>
-      <c r="F22" s="157">
+      <c r="F22" s="102">
         <v>42857</v>
       </c>
     </row>
@@ -3765,177 +3765,177 @@
       <c r="A23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="93"/>
+      <c r="C23" s="140"/>
+      <c r="D23" s="140"/>
+      <c r="E23" s="140"/>
+      <c r="F23" s="141"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="102" t="s">
+      <c r="A24" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="106"/>
-      <c r="D24" s="106"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="107"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="130"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="103"/>
-      <c r="B25" s="108"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="110"/>
+      <c r="A25" s="126"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="132"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="133"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="103"/>
-      <c r="B26" s="108"/>
-      <c r="C26" s="109"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="110"/>
+      <c r="A26" s="126"/>
+      <c r="B26" s="131"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132"/>
+      <c r="F26" s="133"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="103"/>
-      <c r="B27" s="108"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="110"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="132"/>
+      <c r="F27" s="133"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="103"/>
-      <c r="B28" s="108"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="110"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="132"/>
+      <c r="F28" s="133"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="103"/>
-      <c r="B29" s="108"/>
-      <c r="C29" s="109"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="110"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="133"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="103"/>
-      <c r="B30" s="108"/>
-      <c r="C30" s="109"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="110"/>
+      <c r="A30" s="126"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="133"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="103"/>
-      <c r="B31" s="108"/>
-      <c r="C31" s="109"/>
-      <c r="D31" s="109"/>
-      <c r="E31" s="109"/>
-      <c r="F31" s="110"/>
+      <c r="A31" s="126"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="133"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="103"/>
-      <c r="B32" s="108"/>
-      <c r="C32" s="109"/>
-      <c r="D32" s="109"/>
-      <c r="E32" s="109"/>
-      <c r="F32" s="110"/>
+      <c r="A32" s="126"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="132"/>
+      <c r="D32" s="132"/>
+      <c r="E32" s="132"/>
+      <c r="F32" s="133"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="103"/>
-      <c r="B33" s="108"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="110"/>
+      <c r="A33" s="126"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="132"/>
+      <c r="D33" s="132"/>
+      <c r="E33" s="132"/>
+      <c r="F33" s="133"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="103"/>
-      <c r="B34" s="108"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="110"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="132"/>
+      <c r="D34" s="132"/>
+      <c r="E34" s="132"/>
+      <c r="F34" s="133"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="103"/>
-      <c r="B35" s="108"/>
-      <c r="C35" s="109"/>
-      <c r="D35" s="109"/>
-      <c r="E35" s="109"/>
-      <c r="F35" s="110"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="132"/>
+      <c r="D35" s="132"/>
+      <c r="E35" s="132"/>
+      <c r="F35" s="133"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="103"/>
-      <c r="B36" s="108"/>
-      <c r="C36" s="109"/>
-      <c r="D36" s="109"/>
-      <c r="E36" s="109"/>
-      <c r="F36" s="110"/>
+      <c r="A36" s="126"/>
+      <c r="B36" s="131"/>
+      <c r="C36" s="132"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="133"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="103"/>
-      <c r="B37" s="108"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="109"/>
-      <c r="E37" s="109"/>
-      <c r="F37" s="110"/>
+      <c r="A37" s="126"/>
+      <c r="B37" s="131"/>
+      <c r="C37" s="132"/>
+      <c r="D37" s="132"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="133"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="103"/>
-      <c r="B38" s="108"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="109"/>
-      <c r="E38" s="109"/>
-      <c r="F38" s="110"/>
+      <c r="A38" s="126"/>
+      <c r="B38" s="131"/>
+      <c r="C38" s="132"/>
+      <c r="D38" s="132"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="133"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="103"/>
-      <c r="B39" s="108"/>
-      <c r="C39" s="109"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="109"/>
-      <c r="F39" s="110"/>
+      <c r="A39" s="126"/>
+      <c r="B39" s="131"/>
+      <c r="C39" s="132"/>
+      <c r="D39" s="132"/>
+      <c r="E39" s="132"/>
+      <c r="F39" s="133"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="103"/>
-      <c r="B40" s="108"/>
-      <c r="C40" s="109"/>
-      <c r="D40" s="109"/>
-      <c r="E40" s="109"/>
-      <c r="F40" s="110"/>
+      <c r="A40" s="126"/>
+      <c r="B40" s="131"/>
+      <c r="C40" s="132"/>
+      <c r="D40" s="132"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="133"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="103"/>
-      <c r="B41" s="108"/>
-      <c r="C41" s="109"/>
-      <c r="D41" s="109"/>
-      <c r="E41" s="109"/>
-      <c r="F41" s="110"/>
+      <c r="A41" s="126"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="132"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="132"/>
+      <c r="F41" s="133"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="104"/>
-      <c r="B42" s="111"/>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="113"/>
+      <c r="A42" s="127"/>
+      <c r="B42" s="134"/>
+      <c r="C42" s="135"/>
+      <c r="D42" s="135"/>
+      <c r="E42" s="135"/>
+      <c r="F42" s="136"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="94" t="s">
+      <c r="A43" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="94"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="94"/>
-      <c r="E43" s="94"/>
-      <c r="F43" s="94"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="117"/>
+      <c r="E43" s="117"/>
+      <c r="F43" s="117"/>
     </row>
     <row r="44" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="23" t="s">
@@ -3956,241 +3956,252 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="138">
+      <c r="A45" s="83">
         <v>1</v>
       </c>
-      <c r="B45" s="132" t="s">
+      <c r="B45" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="132" t="s">
+      <c r="C45" s="78" t="s">
         <v>179</v>
       </c>
-      <c r="D45" s="132" t="s">
+      <c r="D45" s="78" t="s">
         <v>180</v>
       </c>
-      <c r="E45" s="132" t="s">
+      <c r="E45" s="78" t="s">
         <v>181</v>
       </c>
-      <c r="F45" s="139" t="s">
+      <c r="F45" s="84" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="140">
+      <c r="A46" s="85">
         <v>2</v>
       </c>
-      <c r="B46" s="134" t="s">
+      <c r="B46" s="80" t="s">
         <v>183</v>
       </c>
-      <c r="C46" s="134" t="s">
+      <c r="C46" s="80" t="s">
         <v>185</v>
       </c>
-      <c r="D46" s="137" t="s">
+      <c r="D46" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="E46" s="133" t="s">
+      <c r="E46" s="79" t="s">
         <v>187</v>
       </c>
-      <c r="F46" s="141" t="s">
+      <c r="F46" s="86" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="140"/>
-      <c r="B47" s="134"/>
-      <c r="C47" s="134"/>
-      <c r="D47" s="134"/>
-      <c r="E47" s="134"/>
-      <c r="F47" s="141"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="80"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="86"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="140"/>
-      <c r="B48" s="134"/>
-      <c r="C48" s="134"/>
-      <c r="D48" s="134"/>
-      <c r="E48" s="134"/>
-      <c r="F48" s="141"/>
+      <c r="A48" s="85"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="86"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="142"/>
-      <c r="B49" s="135"/>
-      <c r="C49" s="135"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="135"/>
-      <c r="F49" s="143"/>
+      <c r="A49" s="87"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="88"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="136" t="s">
+      <c r="A52" s="116" t="s">
         <v>184</v>
       </c>
-      <c r="B52" s="131"/>
-      <c r="C52" s="131"/>
-      <c r="D52" s="131"/>
-      <c r="E52" s="131"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="115"/>
+      <c r="D52" s="115"/>
+      <c r="E52" s="115"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="136"/>
-      <c r="B53" s="131"/>
-      <c r="C53" s="131"/>
-      <c r="D53" s="131"/>
-      <c r="E53" s="131"/>
+      <c r="A53" s="116"/>
+      <c r="B53" s="115"/>
+      <c r="C53" s="115"/>
+      <c r="D53" s="115"/>
+      <c r="E53" s="115"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="136"/>
-      <c r="B54" s="131"/>
-      <c r="C54" s="131"/>
-      <c r="D54" s="131"/>
-      <c r="E54" s="131"/>
+      <c r="A54" s="116"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="115"/>
+      <c r="D54" s="115"/>
+      <c r="E54" s="115"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="136"/>
-      <c r="B55" s="131"/>
-      <c r="C55" s="131"/>
-      <c r="D55" s="131"/>
-      <c r="E55" s="131"/>
+      <c r="A55" s="116"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="115"/>
+      <c r="D55" s="115"/>
+      <c r="E55" s="115"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="136"/>
-      <c r="B56" s="131"/>
-      <c r="C56" s="131"/>
-      <c r="D56" s="131"/>
-      <c r="E56" s="131"/>
+      <c r="A56" s="116"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="115"/>
+      <c r="D56" s="115"/>
+      <c r="E56" s="115"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="136"/>
-      <c r="B57" s="131"/>
-      <c r="C57" s="131"/>
-      <c r="D57" s="131"/>
-      <c r="E57" s="131"/>
+      <c r="A57" s="116"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="115"/>
+      <c r="D57" s="115"/>
+      <c r="E57" s="115"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="136"/>
-      <c r="B58" s="131"/>
-      <c r="C58" s="131"/>
-      <c r="D58" s="131"/>
-      <c r="E58" s="131"/>
+      <c r="A58" s="116"/>
+      <c r="B58" s="115"/>
+      <c r="C58" s="115"/>
+      <c r="D58" s="115"/>
+      <c r="E58" s="115"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="136"/>
-      <c r="B59" s="131"/>
-      <c r="C59" s="131"/>
-      <c r="D59" s="131"/>
-      <c r="E59" s="131"/>
+      <c r="A59" s="116"/>
+      <c r="B59" s="115"/>
+      <c r="C59" s="115"/>
+      <c r="D59" s="115"/>
+      <c r="E59" s="115"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="136"/>
-      <c r="B60" s="131"/>
-      <c r="C60" s="131"/>
-      <c r="D60" s="131"/>
-      <c r="E60" s="131"/>
+      <c r="A60" s="116"/>
+      <c r="B60" s="115"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="115"/>
+      <c r="E60" s="115"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="136"/>
-      <c r="B61" s="131"/>
-      <c r="C61" s="131"/>
-      <c r="D61" s="131"/>
-      <c r="E61" s="131"/>
+      <c r="A61" s="116"/>
+      <c r="B61" s="115"/>
+      <c r="C61" s="115"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="115"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="136"/>
-      <c r="B62" s="131"/>
-      <c r="C62" s="131"/>
-      <c r="D62" s="131"/>
-      <c r="E62" s="131"/>
+      <c r="A62" s="116"/>
+      <c r="B62" s="115"/>
+      <c r="C62" s="115"/>
+      <c r="D62" s="115"/>
+      <c r="E62" s="115"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="136"/>
-      <c r="B63" s="131"/>
-      <c r="C63" s="131"/>
-      <c r="D63" s="131"/>
-      <c r="E63" s="131"/>
+      <c r="A63" s="116"/>
+      <c r="B63" s="115"/>
+      <c r="C63" s="115"/>
+      <c r="D63" s="115"/>
+      <c r="E63" s="115"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="136"/>
-      <c r="B64" s="131"/>
-      <c r="C64" s="131"/>
-      <c r="D64" s="131"/>
-      <c r="E64" s="131"/>
+      <c r="A64" s="116"/>
+      <c r="B64" s="115"/>
+      <c r="C64" s="115"/>
+      <c r="D64" s="115"/>
+      <c r="E64" s="115"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="136"/>
-      <c r="B65" s="131"/>
-      <c r="C65" s="131"/>
-      <c r="D65" s="131"/>
-      <c r="E65" s="131"/>
+      <c r="A65" s="116"/>
+      <c r="B65" s="115"/>
+      <c r="C65" s="115"/>
+      <c r="D65" s="115"/>
+      <c r="E65" s="115"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="136"/>
-      <c r="B66" s="131"/>
-      <c r="C66" s="131"/>
-      <c r="D66" s="131"/>
-      <c r="E66" s="131"/>
+      <c r="A66" s="116"/>
+      <c r="B66" s="115"/>
+      <c r="C66" s="115"/>
+      <c r="D66" s="115"/>
+      <c r="E66" s="115"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="136"/>
-      <c r="B67" s="131"/>
-      <c r="C67" s="131"/>
-      <c r="D67" s="131"/>
-      <c r="E67" s="131"/>
+      <c r="A67" s="116"/>
+      <c r="B67" s="115"/>
+      <c r="C67" s="115"/>
+      <c r="D67" s="115"/>
+      <c r="E67" s="115"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="136"/>
-      <c r="B68" s="131"/>
-      <c r="C68" s="131"/>
-      <c r="D68" s="131"/>
-      <c r="E68" s="131"/>
+      <c r="A68" s="116"/>
+      <c r="B68" s="115"/>
+      <c r="C68" s="115"/>
+      <c r="D68" s="115"/>
+      <c r="E68" s="115"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="136"/>
-      <c r="B69" s="131"/>
-      <c r="C69" s="131"/>
-      <c r="D69" s="131"/>
-      <c r="E69" s="131"/>
+      <c r="A69" s="116"/>
+      <c r="B69" s="115"/>
+      <c r="C69" s="115"/>
+      <c r="D69" s="115"/>
+      <c r="E69" s="115"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="136"/>
-      <c r="B70" s="131"/>
-      <c r="C70" s="131"/>
-      <c r="D70" s="131"/>
-      <c r="E70" s="131"/>
+      <c r="A70" s="116"/>
+      <c r="B70" s="115"/>
+      <c r="C70" s="115"/>
+      <c r="D70" s="115"/>
+      <c r="E70" s="115"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="136"/>
-      <c r="B71" s="131"/>
-      <c r="C71" s="131"/>
-      <c r="D71" s="131"/>
-      <c r="E71" s="131"/>
+      <c r="A71" s="116"/>
+      <c r="B71" s="115"/>
+      <c r="C71" s="115"/>
+      <c r="D71" s="115"/>
+      <c r="E71" s="115"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="136"/>
-      <c r="B72" s="131"/>
-      <c r="C72" s="131"/>
-      <c r="D72" s="131"/>
-      <c r="E72" s="131"/>
+      <c r="A72" s="116"/>
+      <c r="B72" s="115"/>
+      <c r="C72" s="115"/>
+      <c r="D72" s="115"/>
+      <c r="E72" s="115"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="136"/>
-      <c r="B73" s="131"/>
-      <c r="C73" s="131"/>
-      <c r="D73" s="131"/>
-      <c r="E73" s="131"/>
+      <c r="A73" s="116"/>
+      <c r="B73" s="115"/>
+      <c r="C73" s="115"/>
+      <c r="D73" s="115"/>
+      <c r="E73" s="115"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="136"/>
-      <c r="B74" s="131"/>
-      <c r="C74" s="131"/>
-      <c r="D74" s="131"/>
-      <c r="E74" s="131"/>
+      <c r="A74" s="116"/>
+      <c r="B74" s="115"/>
+      <c r="C74" s="115"/>
+      <c r="D74" s="115"/>
+      <c r="E74" s="115"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="136"/>
-      <c r="B75" s="131"/>
-      <c r="C75" s="131"/>
-      <c r="D75" s="131"/>
-      <c r="E75" s="131"/>
+      <c r="A75" s="116"/>
+      <c r="B75" s="115"/>
+      <c r="C75" s="115"/>
+      <c r="D75" s="115"/>
+      <c r="E75" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="B52:E75"/>
     <mergeCell ref="A52:A75"/>
     <mergeCell ref="A43:F43"/>
@@ -4200,17 +4211,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="A24:A42"/>
     <mergeCell ref="B24:F42"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D13:D22">
     <cfRule type="cellIs" dxfId="69" priority="5" stopIfTrue="1" operator="equal">
@@ -4260,8 +4260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G6"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4281,169 +4281,169 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="90">
+      <c r="B1" s="137">
         <v>302</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="139" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="137"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="138" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="138"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="130">
+      <c r="B6" s="142">
         <v>42857</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
+      <c r="G6" s="138"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="137"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="151" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="114"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="114"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
+      <c r="G11" s="151"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="D12" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="99" t="s">
+      <c r="E12" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="100"/>
-      <c r="G12" s="101"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="124"/>
     </row>
     <row r="13" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116"/>
-      <c r="B13" s="117"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="98"/>
+      <c r="A13" s="144"/>
+      <c r="B13" s="145"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="121"/>
       <c r="E13" s="32" t="s">
         <v>17</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>7</v>
       </c>
       <c r="F14" s="39"/>
-      <c r="G14" s="158">
+      <c r="G14" s="103">
         <v>42857</v>
       </c>
     </row>
@@ -4486,7 +4486,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="42"/>
-      <c r="G15" s="154">
+      <c r="G15" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4505,7 +4505,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="42"/>
-      <c r="G16" s="154">
+      <c r="G16" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4526,7 +4526,7 @@
       <c r="F17" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="G17" s="154">
+      <c r="G17" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4545,7 +4545,7 @@
         <v>7</v>
       </c>
       <c r="F18" s="42"/>
-      <c r="G18" s="154">
+      <c r="G18" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4561,10 +4561,10 @@
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="41" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F19" s="42"/>
-      <c r="G19" s="154">
+      <c r="G19" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4581,7 +4581,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="42"/>
-      <c r="G20" s="154">
+      <c r="G20" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4600,7 +4600,7 @@
         <v>7</v>
       </c>
       <c r="F21" s="42"/>
-      <c r="G21" s="154">
+      <c r="G21" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4619,7 +4619,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="42"/>
-      <c r="G22" s="154">
+      <c r="G22" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4635,10 +4635,10 @@
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="41" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F23" s="42"/>
-      <c r="G23" s="154">
+      <c r="G23" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4655,7 +4655,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="42"/>
-      <c r="G24" s="154">
+      <c r="G24" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
         <v>7</v>
       </c>
       <c r="F25" s="42"/>
-      <c r="G25" s="154">
+      <c r="G25" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4691,7 +4691,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="42"/>
-      <c r="G26" s="154">
+      <c r="G26" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4710,7 +4710,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="42"/>
-      <c r="G27" s="154">
+      <c r="G27" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -4729,7 +4729,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="47"/>
-      <c r="G28" s="157">
+      <c r="G28" s="102">
         <v>42857</v>
       </c>
     </row>
@@ -4737,27 +4737,27 @@
       <c r="A29" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="92"/>
-      <c r="D29" s="92"/>
-      <c r="E29" s="92"/>
-      <c r="F29" s="92"/>
-      <c r="G29" s="93"/>
+      <c r="C29" s="140"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="141"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="120" t="s">
+      <c r="B30" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="121"/>
-      <c r="E30" s="121"/>
-      <c r="F30" s="121"/>
-      <c r="G30" s="122"/>
+      <c r="C30" s="149"/>
+      <c r="D30" s="149"/>
+      <c r="E30" s="149"/>
+      <c r="F30" s="149"/>
+      <c r="G30" s="150"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21"/>
@@ -4769,15 +4769,15 @@
       <c r="G31" s="22"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="143" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="115"/>
-      <c r="C32" s="115"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
+      <c r="B32" s="143"/>
+      <c r="C32" s="143"/>
+      <c r="D32" s="143"/>
+      <c r="E32" s="143"/>
+      <c r="F32" s="143"/>
+      <c r="G32" s="143"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="23" t="s">
@@ -4847,6 +4847,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
@@ -4854,18 +4866,6 @@
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="E14:E28">
     <cfRule type="cellIs" dxfId="60" priority="9" stopIfTrue="1" operator="equal">
@@ -4914,8 +4914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:F6"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,154 +4933,154 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="90">
+      <c r="B1" s="137">
         <v>303</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="139" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="138" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="130">
+      <c r="B6" s="142">
         <v>42857</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="151" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="114"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="99" t="s">
+      <c r="D12" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="100"/>
-      <c r="F12" s="101"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="124"/>
     </row>
     <row r="13" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="96"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="123"/>
+      <c r="A13" s="119"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="152"/>
       <c r="D13" s="33" t="s">
         <v>17</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="39"/>
-      <c r="F14" s="158">
+      <c r="F14" s="103">
         <v>42857</v>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="42"/>
-      <c r="F15" s="154">
+      <c r="F15" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="42"/>
-      <c r="F16" s="154">
+      <c r="F16" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -5153,7 +5153,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="42"/>
-      <c r="F17" s="154">
+      <c r="F17" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -5171,7 +5171,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="29"/>
-      <c r="F18" s="155">
+      <c r="F18" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -5179,25 +5179,25 @@
       <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
-      <c r="F19" s="122"/>
+      <c r="C19" s="149"/>
+      <c r="D19" s="149"/>
+      <c r="E19" s="149"/>
+      <c r="F19" s="150"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="120" t="s">
+      <c r="B20" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
-      <c r="F20" s="122"/>
+      <c r="C20" s="149"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="149"/>
+      <c r="F20" s="150"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
@@ -5208,14 +5208,14 @@
       <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="115" t="s">
+      <c r="A22" s="143" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="115"/>
-      <c r="C22" s="115"/>
-      <c r="D22" s="115"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="115"/>
+      <c r="B22" s="143"/>
+      <c r="C22" s="143"/>
+      <c r="D22" s="143"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="143"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
@@ -5279,24 +5279,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B11:F11"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:D18">
     <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
@@ -5345,8 +5345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:F6"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5365,154 +5365,154 @@
       <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="90">
+      <c r="B1" s="137">
         <v>304</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="139" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="138" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="130">
+      <c r="B6" s="142">
         <v>42857</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="138" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
+      <c r="C8" s="138"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="139" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
+      <c r="C10" s="138"/>
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="151" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="114"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="114"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="97" t="s">
+      <c r="B12" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="99" t="s">
+      <c r="D12" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="100"/>
-      <c r="F12" s="101"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="124"/>
     </row>
     <row r="13" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="96"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="123"/>
+      <c r="A13" s="119"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="152"/>
       <c r="D13" s="33" t="s">
         <v>17</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="42"/>
-      <c r="F14" s="154">
+      <c r="F14" s="99">
         <v>42857</v>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="29"/>
-      <c r="F15" s="155">
+      <c r="F15" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -5569,7 +5569,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="29"/>
-      <c r="F16" s="155">
+      <c r="F16" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="29"/>
-      <c r="F17" s="155">
+      <c r="F17" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -5605,7 +5605,7 @@
         <v>7</v>
       </c>
       <c r="E18" s="29"/>
-      <c r="F18" s="155">
+      <c r="F18" s="100">
         <v>42857</v>
       </c>
     </row>
@@ -5623,7 +5623,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="53"/>
-      <c r="F19" s="156">
+      <c r="F19" s="101">
         <v>42857</v>
       </c>
     </row>
@@ -5641,7 +5641,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="47"/>
-      <c r="F20" s="157">
+      <c r="F20" s="102">
         <v>42857</v>
       </c>
     </row>
@@ -5649,25 +5649,25 @@
       <c r="A21" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="121" t="s">
+      <c r="B21" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="121"/>
-      <c r="D21" s="121"/>
-      <c r="E21" s="121"/>
-      <c r="F21" s="122"/>
+      <c r="C21" s="149"/>
+      <c r="D21" s="149"/>
+      <c r="E21" s="149"/>
+      <c r="F21" s="150"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="120" t="s">
+      <c r="B22" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
-      <c r="E22" s="121"/>
-      <c r="F22" s="122"/>
+      <c r="C22" s="149"/>
+      <c r="D22" s="149"/>
+      <c r="E22" s="149"/>
+      <c r="F22" s="150"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
@@ -5678,14 +5678,14 @@
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="115" t="s">
+      <c r="A24" s="143" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="115"/>
-      <c r="C24" s="115"/>
-      <c r="D24" s="115"/>
-      <c r="E24" s="115"/>
-      <c r="F24" s="115"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="143"/>
+      <c r="E24" s="143"/>
+      <c r="F24" s="143"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
@@ -5749,24 +5749,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B11:F11"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:D20">
     <cfRule type="cellIs" dxfId="42" priority="5" stopIfTrue="1" operator="equal">
@@ -5815,8 +5815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5839,164 +5839,164 @@
       <c r="A1" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="137"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="137"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="138"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="139" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="139"/>
+      <c r="L5" s="139"/>
+      <c r="M5" s="139"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="155" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="126"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="155"/>
+      <c r="G6" s="155"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="155"/>
+      <c r="J6" s="155"/>
+      <c r="K6" s="155"/>
+      <c r="L6" s="155"/>
+      <c r="M6" s="155"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="118" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="153" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="124" t="s">
+      <c r="D7" s="153" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="124" t="s">
+      <c r="E7" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="124" t="s">
+      <c r="F7" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="97" t="s">
+      <c r="I7" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="118" t="s">
+      <c r="J7" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="99" t="s">
+      <c r="K7" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="100"/>
-      <c r="M7" s="101"/>
+      <c r="L7" s="123"/>
+      <c r="M7" s="124"/>
     </row>
     <row r="8" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="96"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="123"/>
+      <c r="A8" s="119"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
+      <c r="E8" s="154"/>
+      <c r="F8" s="154"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="152"/>
       <c r="K8" s="33" t="s">
         <v>97</v>
       </c>
@@ -6017,7 +6017,7 @@
       <c r="C9" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="D9" s="144">
+      <c r="D9" s="89">
         <v>42857</v>
       </c>
       <c r="E9" s="61" t="s">
@@ -6038,7 +6038,7 @@
         <v>7</v>
       </c>
       <c r="L9" s="37"/>
-      <c r="M9" s="149">
+      <c r="M9" s="94">
         <v>42857</v>
       </c>
     </row>
@@ -6052,7 +6052,7 @@
       <c r="C10" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="D10" s="150">
+      <c r="D10" s="95">
         <v>42857</v>
       </c>
       <c r="E10" s="57" t="s">
@@ -6079,7 +6079,7 @@
       <c r="L10" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="M10" s="147">
+      <c r="M10" s="92">
         <v>42857</v>
       </c>
     </row>
@@ -6093,7 +6093,7 @@
       <c r="C11" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="D11" s="150">
+      <c r="D11" s="95">
         <v>42857</v>
       </c>
       <c r="E11" s="57" t="s">
@@ -6114,7 +6114,7 @@
         <v>7</v>
       </c>
       <c r="L11" s="34"/>
-      <c r="M11" s="147">
+      <c r="M11" s="92">
         <v>42857</v>
       </c>
     </row>
@@ -6128,7 +6128,7 @@
       <c r="C12" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="D12" s="150">
+      <c r="D12" s="95">
         <v>42857</v>
       </c>
       <c r="E12" s="57" t="s">
@@ -6151,7 +6151,7 @@
         <v>7</v>
       </c>
       <c r="L12" s="34"/>
-      <c r="M12" s="147">
+      <c r="M12" s="92">
         <v>42857</v>
       </c>
     </row>
@@ -6165,7 +6165,7 @@
       <c r="C13" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="150">
+      <c r="D13" s="95">
         <v>42857</v>
       </c>
       <c r="E13" s="57" t="s">
@@ -6190,7 +6190,7 @@
       <c r="L13" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="M13" s="147">
+      <c r="M13" s="92">
         <v>42857</v>
       </c>
     </row>
@@ -6204,7 +6204,7 @@
       <c r="C14" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="D14" s="153">
+      <c r="D14" s="98">
         <v>42857</v>
       </c>
       <c r="E14" s="74" t="s">
@@ -6229,7 +6229,7 @@
       <c r="L14" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="M14" s="148">
+      <c r="M14" s="93">
         <v>42857</v>
       </c>
     </row>
@@ -6243,7 +6243,7 @@
       <c r="C15" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="144">
+      <c r="D15" s="89">
         <v>42857</v>
       </c>
       <c r="E15" s="61" t="s">
@@ -6266,7 +6266,7 @@
       <c r="L15" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="M15" s="149">
+      <c r="M15" s="94">
         <v>42857</v>
       </c>
     </row>
@@ -6280,7 +6280,7 @@
       <c r="C16" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="150">
+      <c r="D16" s="95">
         <v>42857</v>
       </c>
       <c r="E16" s="57" t="s">
@@ -6301,7 +6301,7 @@
         <v>7</v>
       </c>
       <c r="L16" s="34"/>
-      <c r="M16" s="147">
+      <c r="M16" s="92">
         <v>42857</v>
       </c>
     </row>
@@ -6315,7 +6315,7 @@
       <c r="C17" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="D17" s="152">
+      <c r="D17" s="97">
         <v>42857</v>
       </c>
       <c r="E17" s="63" t="s">
@@ -6338,7 +6338,7 @@
       <c r="L17" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="M17" s="146">
+      <c r="M17" s="91">
         <v>42857</v>
       </c>
     </row>
@@ -6352,7 +6352,7 @@
       <c r="C18" s="64" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="151">
+      <c r="D18" s="96">
         <v>42857</v>
       </c>
       <c r="E18" s="64" t="s">
@@ -6375,12 +6375,13 @@
       <c r="L18" s="64" t="s">
         <v>192</v>
       </c>
-      <c r="M18" s="145">
+      <c r="M18" s="90">
         <v>42857</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="B5:M5"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
@@ -6397,7 +6398,6 @@
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="K9:K18">
     <cfRule type="cellIs" dxfId="33" priority="5" stopIfTrue="1" operator="equal">
@@ -6456,111 +6456,111 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="156" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="127"/>
-      <c r="P1" s="127"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="156"/>
+      <c r="L1" s="156"/>
+      <c r="M1" s="156"/>
+      <c r="N1" s="156"/>
+      <c r="O1" s="156"/>
+      <c r="P1" s="156"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="157" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="157"/>
+      <c r="I2" s="157"/>
+      <c r="J2" s="157"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="157"/>
+      <c r="M2" s="157"/>
+      <c r="N2" s="157"/>
+      <c r="O2" s="157"/>
+      <c r="P2" s="157"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="129"/>
-      <c r="O3" s="129"/>
-      <c r="P3" s="129"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
+      <c r="L3" s="158"/>
+      <c r="M3" s="158"/>
+      <c r="N3" s="158"/>
+      <c r="O3" s="158"/>
+      <c r="P3" s="158"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="157" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="128"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="157"/>
+      <c r="E4" s="157"/>
+      <c r="F4" s="157"/>
+      <c r="G4" s="157"/>
+      <c r="H4" s="157"/>
+      <c r="I4" s="157"/>
+      <c r="J4" s="157"/>
+      <c r="K4" s="157"/>
+      <c r="L4" s="157"/>
+      <c r="M4" s="157"/>
+      <c r="N4" s="157"/>
+      <c r="O4" s="157"/>
+      <c r="P4" s="157"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="127"/>
-      <c r="D5" s="127"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127"/>
-      <c r="P5" s="127"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
+      <c r="H5" s="156"/>
+      <c r="I5" s="156"/>
+      <c r="J5" s="156"/>
+      <c r="K5" s="156"/>
+      <c r="L5" s="156"/>
+      <c r="M5" s="156"/>
+      <c r="N5" s="156"/>
+      <c r="O5" s="156"/>
+      <c r="P5" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>